<commit_message>
Still need to figure out Kuva/Tenet adjustments.
</commit_message>
<xml_diff>
--- a/DamageCalcs/DMG-Calc.xlsx
+++ b/DamageCalcs/DMG-Calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WarframeDamage\WF-DataImporter\DamageCalcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC07AD7-F5A7-4E80-9EC4-60D47CAA4CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D780C-B86F-4D76-AD94-58EF83AB1AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{EB71189C-B0E1-4425-AB4D-84E53115CCBD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{EB71189C-B0E1-4425-AB4D-84E53115CCBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="822">
   <si>
     <t>Latron Prime</t>
   </si>
@@ -2523,6 +2523,9 @@
   </si>
   <si>
     <t>removed from row</t>
+  </si>
+  <si>
+    <t>XLOOKUP([@WEAPON],WeaponData[WEAPON],WeaponData[ELEC],0)</t>
   </si>
 </sst>
 </file>
@@ -2804,6 +2807,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2864,9 +2870,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2885,667 +2888,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4181,6 +3534,681 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -8217,21 +8245,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="16"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -8257,56 +8270,56 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3A90822B-393F-4049-A399-753E70DCCA96}" name="BaseValues" displayName="BaseValues" ref="A3:R4" headerRowDxfId="305" dataDxfId="304">
   <autoFilter ref="A3:R4" xr:uid="{3A90822B-393F-4049-A399-753E70DCCA96}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{480EAED2-C7A5-4D36-9D6E-17AC741D81F6}" name="WEAPON" dataDxfId="303" totalsRowDxfId="302"/>
-    <tableColumn id="2" xr3:uid="{0D944825-FE74-4F70-B006-3A17ADFDFF23}" name="QUANTA" dataDxfId="301" totalsRowDxfId="300">
+    <tableColumn id="1" xr3:uid="{480EAED2-C7A5-4D36-9D6E-17AC741D81F6}" name="WEAPON" dataDxfId="0" totalsRowDxfId="303"/>
+    <tableColumn id="2" xr3:uid="{0D944825-FE74-4F70-B006-3A17ADFDFF23}" name="QUANTA" dataDxfId="302" totalsRowDxfId="301">
       <calculatedColumnFormula>BaseValues[[#This Row],[TOTAL]]/16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CC66DE8B-0DBC-486A-900A-51E3C9793CEF}" name="IMPACT" dataDxfId="299" totalsRowDxfId="298">
+    <tableColumn id="3" xr3:uid="{CC66DE8B-0DBC-486A-900A-51E3C9793CEF}" name="IMPACT" dataDxfId="300" totalsRowDxfId="299">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[IMPACT],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3131F927-7E6B-4AE6-8ABB-5A7E1D1668F6}" name="PUNC" dataDxfId="297" totalsRowDxfId="296">
+    <tableColumn id="4" xr3:uid="{3131F927-7E6B-4AE6-8ABB-5A7E1D1668F6}" name="PUNC" dataDxfId="298" totalsRowDxfId="297">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[PUNC],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F2B5E26A-E038-49C0-958A-756017C34492}" name="SLASH" dataDxfId="295" totalsRowDxfId="294">
+    <tableColumn id="5" xr3:uid="{F2B5E26A-E038-49C0-958A-756017C34492}" name="SLASH" dataDxfId="296" totalsRowDxfId="295">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[SLASH],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{721C2421-5FAF-4E69-B0A3-5F078DD41796}" name="HEAT" dataDxfId="293" totalsRowDxfId="292">
+    <tableColumn id="6" xr3:uid="{721C2421-5FAF-4E69-B0A3-5F078DD41796}" name="HEAT" dataDxfId="294" totalsRowDxfId="293">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[HEAT],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{75496494-478C-483A-8F62-7A3D5277E75F}" name="COLD" dataDxfId="291" totalsRowDxfId="290">
+    <tableColumn id="7" xr3:uid="{75496494-478C-483A-8F62-7A3D5277E75F}" name="COLD" dataDxfId="292" totalsRowDxfId="291">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[COLD],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{309D4709-0D36-4191-A5A5-6C8045D4F2B5}" name="ELEC" dataDxfId="289" totalsRowDxfId="288">
+    <tableColumn id="8" xr3:uid="{309D4709-0D36-4191-A5A5-6C8045D4F2B5}" name="ELEC" dataDxfId="290" totalsRowDxfId="289">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[ELEC],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ED125659-FE3E-494D-AEE4-DEEBFA0C570C}" name="TOXIN" dataDxfId="287" totalsRowDxfId="286">
+    <tableColumn id="9" xr3:uid="{ED125659-FE3E-494D-AEE4-DEEBFA0C570C}" name="TOXIN" dataDxfId="288" totalsRowDxfId="287">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[TOXIN],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{674EE424-CAEA-4644-8FEF-783CBB3DC6C7}" name="BLAST" dataDxfId="285" totalsRowDxfId="284">
+    <tableColumn id="12" xr3:uid="{674EE424-CAEA-4644-8FEF-783CBB3DC6C7}" name="BLAST" dataDxfId="286" totalsRowDxfId="285">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[BLAST],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{DF70299C-5C96-4411-9C8C-99C3B18F5A8D}" name="RAD" dataDxfId="283" totalsRowDxfId="282">
+    <tableColumn id="16" xr3:uid="{DF70299C-5C96-4411-9C8C-99C3B18F5A8D}" name="RAD" dataDxfId="284" totalsRowDxfId="283">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[RAD],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{46AE3FDE-0B2C-4C8E-9561-EA42FF8091B1}" name="GAS" dataDxfId="281" totalsRowDxfId="280">
+    <tableColumn id="14" xr3:uid="{46AE3FDE-0B2C-4C8E-9561-EA42FF8091B1}" name="GAS" dataDxfId="282" totalsRowDxfId="281">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[GAS],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{56AA859D-AD50-41FC-B6D1-77B139205600}" name="MAG" dataDxfId="279" totalsRowDxfId="278">
+    <tableColumn id="15" xr3:uid="{56AA859D-AD50-41FC-B6D1-77B139205600}" name="MAG" dataDxfId="280" totalsRowDxfId="279">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[MAG],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{6D015471-048E-424D-997E-E6D9B839B49A}" name="VIRAL" dataDxfId="277" totalsRowDxfId="276">
+    <tableColumn id="17" xr3:uid="{6D015471-048E-424D-997E-E6D9B839B49A}" name="VIRAL" dataDxfId="278" totalsRowDxfId="277">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[VIRAL],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A7FF00A7-4D37-4253-8508-2AC03C464FE6}" name="CORR" dataDxfId="275" totalsRowDxfId="274">
+    <tableColumn id="13" xr3:uid="{A7FF00A7-4D37-4253-8508-2AC03C464FE6}" name="CORR" dataDxfId="276" totalsRowDxfId="275">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[CORR],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{CA7D12EF-1742-4627-8108-03659E5F3EEA}" name="VOID" dataDxfId="273" totalsRowDxfId="272">
+    <tableColumn id="10" xr3:uid="{CA7D12EF-1742-4627-8108-03659E5F3EEA}" name="VOID" dataDxfId="274" totalsRowDxfId="273">
       <calculatedColumnFormula>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[VOID],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7E1E9929-0FBC-4207-8B80-F3C8EAC2A92C}" name="TOTAL" dataDxfId="271" totalsRowDxfId="270">
+    <tableColumn id="18" xr3:uid="{7E1E9929-0FBC-4207-8B80-F3C8EAC2A92C}" name="TOTAL" dataDxfId="272" totalsRowDxfId="271">
       <calculatedColumnFormula>SUM(BaseValues[[#This Row],[IMPACT]:[VOID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F9AAC047-B8B4-4E8F-8F0F-348623281921}" name="RTOTAL" dataDxfId="269" totalsRowDxfId="268">
+    <tableColumn id="11" xr3:uid="{F9AAC047-B8B4-4E8F-8F0F-348623281921}" name="RTOTAL" dataDxfId="270" totalsRowDxfId="269">
       <calculatedColumnFormula>ROUND(BaseValues[[#This Row],[TOTAL]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8315,216 +8328,208 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DBD27117-B79D-4E40-9835-D353C0C6E1AA}" name="ModValues" displayName="ModValues" ref="A7:R8" headerRowDxfId="267" dataDxfId="266">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DBD27117-B79D-4E40-9835-D353C0C6E1AA}" name="ModValues" displayName="ModValues" ref="A7:R8" headerRowDxfId="268" dataDxfId="267">
   <autoFilter ref="A7:R8" xr:uid="{DBD27117-B79D-4E40-9835-D353C0C6E1AA}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{529A0FD5-F34F-40B0-B961-CBAD530BD7CB}" name="WEAPON" dataDxfId="265" totalsRowDxfId="264">
-      <calculatedColumnFormula array="1">BaseValues[WEAPON]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{A7692FE2-B64E-48A3-BC5C-17DA27FF06BA}" name="QUANTA" dataDxfId="263" totalsRowDxfId="262">
+    <tableColumn id="1" xr3:uid="{529A0FD5-F34F-40B0-B961-CBAD530BD7CB}" name="WEAPON" dataDxfId="266" totalsRowDxfId="265"/>
+    <tableColumn id="2" xr3:uid="{A7692FE2-B64E-48A3-BC5C-17DA27FF06BA}" name="QUANTA" dataDxfId="264" totalsRowDxfId="263">
       <calculatedColumnFormula array="1">ROUND(BaseValues[QUANTA],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C4A903CA-AAA8-4EF6-B25B-8C836F01631F}" name="IMPACT" dataDxfId="261" totalsRowDxfId="260"/>
-    <tableColumn id="4" xr3:uid="{AAE8B413-770B-4E89-A313-EA350BD4A3E4}" name="PUNC" dataDxfId="259" totalsRowDxfId="258">
-      <calculatedColumnFormula>1.2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{11EABA99-2A29-4C7F-84D9-D9A2D96B55E1}" name="SLASH" dataDxfId="257" totalsRowDxfId="256"/>
-    <tableColumn id="6" xr3:uid="{84D7162E-7FEF-404F-BF4A-3B7A4B7ED6DD}" name="HEAT" dataDxfId="255" totalsRowDxfId="254"/>
-    <tableColumn id="7" xr3:uid="{052B6454-13AA-4C50-A9D8-0CC7E9CD641E}" name="COLD" dataDxfId="253" totalsRowDxfId="252"/>
-    <tableColumn id="8" xr3:uid="{A2EA1F2A-9869-4DD7-8F7A-0825C933B7F7}" name="ELEC" dataDxfId="251" totalsRowDxfId="250"/>
-    <tableColumn id="9" xr3:uid="{BA6CCDCD-09A3-4D8D-A2C4-8698AE5E4636}" name="TOXIN" dataDxfId="249" totalsRowDxfId="248"/>
-    <tableColumn id="12" xr3:uid="{C95C9C6B-A60F-45F3-97F1-CEC8D900634C}" name="BLAST" dataDxfId="247" totalsRowDxfId="246"/>
-    <tableColumn id="16" xr3:uid="{56722A68-1E3A-4DE8-ADC2-B71B4350E862}" name="RAD" dataDxfId="245" totalsRowDxfId="244"/>
-    <tableColumn id="14" xr3:uid="{56F3584A-EA87-4E02-8FE8-B726026F29E5}" name="GAS" dataDxfId="243" totalsRowDxfId="242"/>
-    <tableColumn id="15" xr3:uid="{5864FC43-9D2E-4019-B834-31907DC7D950}" name="MAG" dataDxfId="241" totalsRowDxfId="240">
-      <calculatedColumnFormula>0.9+0.9</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{C9BCB6FF-C065-4BA8-ABDA-56DA218EABE8}" name="VIRAL" dataDxfId="239" totalsRowDxfId="238"/>
-    <tableColumn id="13" xr3:uid="{D5D8398F-2F0D-4E27-8680-49FACEB5957A}" name="CORR" dataDxfId="237" totalsRowDxfId="236"/>
-    <tableColumn id="10" xr3:uid="{975DFB64-F9FD-4099-95BF-E3092C6B22BB}" name="VOID" dataDxfId="235" totalsRowDxfId="234"/>
-    <tableColumn id="18" xr3:uid="{32E28DB2-CDCB-4A77-94C9-342107F1DEE8}" name="TRUE" dataDxfId="233" totalsRowDxfId="232">
-      <calculatedColumnFormula>1.65</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{B92A3A33-90F6-4A23-9B53-AC54E17113D9}" name="BANE" dataDxfId="231" totalsRowDxfId="230"/>
+    <tableColumn id="3" xr3:uid="{C4A903CA-AAA8-4EF6-B25B-8C836F01631F}" name="IMPACT" dataDxfId="262" totalsRowDxfId="261"/>
+    <tableColumn id="4" xr3:uid="{AAE8B413-770B-4E89-A313-EA350BD4A3E4}" name="PUNC" dataDxfId="260" totalsRowDxfId="259"/>
+    <tableColumn id="5" xr3:uid="{11EABA99-2A29-4C7F-84D9-D9A2D96B55E1}" name="SLASH" dataDxfId="258" totalsRowDxfId="257"/>
+    <tableColumn id="6" xr3:uid="{84D7162E-7FEF-404F-BF4A-3B7A4B7ED6DD}" name="HEAT" dataDxfId="256" totalsRowDxfId="255"/>
+    <tableColumn id="7" xr3:uid="{052B6454-13AA-4C50-A9D8-0CC7E9CD641E}" name="COLD" dataDxfId="254" totalsRowDxfId="253"/>
+    <tableColumn id="8" xr3:uid="{A2EA1F2A-9869-4DD7-8F7A-0825C933B7F7}" name="ELEC" dataDxfId="252" totalsRowDxfId="251"/>
+    <tableColumn id="9" xr3:uid="{BA6CCDCD-09A3-4D8D-A2C4-8698AE5E4636}" name="TOXIN" dataDxfId="250" totalsRowDxfId="249"/>
+    <tableColumn id="12" xr3:uid="{C95C9C6B-A60F-45F3-97F1-CEC8D900634C}" name="BLAST" dataDxfId="248" totalsRowDxfId="247"/>
+    <tableColumn id="16" xr3:uid="{56722A68-1E3A-4DE8-ADC2-B71B4350E862}" name="RAD" dataDxfId="246" totalsRowDxfId="245"/>
+    <tableColumn id="14" xr3:uid="{56F3584A-EA87-4E02-8FE8-B726026F29E5}" name="GAS" dataDxfId="244" totalsRowDxfId="243"/>
+    <tableColumn id="15" xr3:uid="{5864FC43-9D2E-4019-B834-31907DC7D950}" name="MAG" dataDxfId="242" totalsRowDxfId="241"/>
+    <tableColumn id="17" xr3:uid="{C9BCB6FF-C065-4BA8-ABDA-56DA218EABE8}" name="VIRAL" dataDxfId="240" totalsRowDxfId="239"/>
+    <tableColumn id="13" xr3:uid="{D5D8398F-2F0D-4E27-8680-49FACEB5957A}" name="CORR" dataDxfId="238" totalsRowDxfId="237"/>
+    <tableColumn id="10" xr3:uid="{975DFB64-F9FD-4099-95BF-E3092C6B22BB}" name="VOID" dataDxfId="236" totalsRowDxfId="235"/>
+    <tableColumn id="18" xr3:uid="{32E28DB2-CDCB-4A77-94C9-342107F1DEE8}" name="TRUE" dataDxfId="234" totalsRowDxfId="233"/>
+    <tableColumn id="11" xr3:uid="{B92A3A33-90F6-4A23-9B53-AC54E17113D9}" name="BANE" dataDxfId="232" totalsRowDxfId="231"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF560950-92C3-4D0A-A7F2-60F81B19C513}" name="ArmorMOD" displayName="ArmorMOD" ref="A15:R16" headerRowDxfId="229" dataDxfId="228">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF560950-92C3-4D0A-A7F2-60F81B19C513}" name="ArmorMOD" displayName="ArmorMOD" ref="A15:R16" headerRowDxfId="230" dataDxfId="229">
   <autoFilter ref="A15:R16" xr:uid="{DF560950-92C3-4D0A-A7F2-60F81B19C513}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{671E3145-786C-4F7D-A446-1EDB990019AE}" name="ARMOR" dataDxfId="227" totalsRowDxfId="226"/>
-    <tableColumn id="2" xr3:uid="{B0B4F0B8-D874-4975-8E6E-B2F4BAFAE573}" name="QUANTA" dataDxfId="225" totalsRowDxfId="224">
+    <tableColumn id="1" xr3:uid="{671E3145-786C-4F7D-A446-1EDB990019AE}" name="ARMOR" dataDxfId="228" totalsRowDxfId="227"/>
+    <tableColumn id="2" xr3:uid="{B0B4F0B8-D874-4975-8E6E-B2F4BAFAE573}" name="QUANTA" dataDxfId="226" totalsRowDxfId="225">
       <calculatedColumnFormula array="1">BaseValues[QUANTA]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{820B1EE7-44D5-454F-B882-E0CA6ADE5009}" name="IMPACT" dataDxfId="223" totalsRowDxfId="222">
+    <tableColumn id="3" xr3:uid="{820B1EE7-44D5-454F-B882-E0CA6ADE5009}" name="IMPACT" dataDxfId="224" totalsRowDxfId="223">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7BD067DC-C3B7-4E7E-B644-08A3D1E308D8}" name="PUNC" dataDxfId="221" totalsRowDxfId="220">
+    <tableColumn id="4" xr3:uid="{7BD067DC-C3B7-4E7E-B644-08A3D1E308D8}" name="PUNC" dataDxfId="222" totalsRowDxfId="221">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D1B78B54-BD2D-402A-900E-A63E2679B302}" name="SLASH" dataDxfId="219" totalsRowDxfId="218">
+    <tableColumn id="5" xr3:uid="{D1B78B54-BD2D-402A-900E-A63E2679B302}" name="SLASH" dataDxfId="220" totalsRowDxfId="219">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A1A37641-5080-4BDA-865D-901B31960187}" name="HEAT" dataDxfId="217" totalsRowDxfId="216">
+    <tableColumn id="6" xr3:uid="{A1A37641-5080-4BDA-865D-901B31960187}" name="HEAT" dataDxfId="218" totalsRowDxfId="217">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{43D72337-DA51-4953-9636-5CB3F71E881E}" name="COLD" dataDxfId="215" totalsRowDxfId="214">
+    <tableColumn id="7" xr3:uid="{43D72337-DA51-4953-9636-5CB3F71E881E}" name="COLD" dataDxfId="216" totalsRowDxfId="215">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{315EA1B2-555C-408D-9DAE-28062A286BD9}" name="ELEC" dataDxfId="213" totalsRowDxfId="212">
+    <tableColumn id="8" xr3:uid="{315EA1B2-555C-408D-9DAE-28062A286BD9}" name="ELEC" dataDxfId="214" totalsRowDxfId="213">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F32CBBBF-DB70-415F-A773-2E7974B6A1C5}" name="TOXIN" dataDxfId="211" totalsRowDxfId="210">
+    <tableColumn id="9" xr3:uid="{F32CBBBF-DB70-415F-A773-2E7974B6A1C5}" name="TOXIN" dataDxfId="212" totalsRowDxfId="211">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{60428664-E2CD-4C78-834F-3B99EB30846E}" name="BLAST" dataDxfId="209" totalsRowDxfId="208">
+    <tableColumn id="12" xr3:uid="{60428664-E2CD-4C78-834F-3B99EB30846E}" name="BLAST" dataDxfId="210" totalsRowDxfId="209">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{D1837C78-78AD-4692-AD44-31C0B068B869}" name="RAD" dataDxfId="207" totalsRowDxfId="206">
+    <tableColumn id="16" xr3:uid="{D1837C78-78AD-4692-AD44-31C0B068B869}" name="RAD" dataDxfId="208" totalsRowDxfId="207">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7DFC35B2-4706-4AE3-A96B-F2996065D7AA}" name="GAS" dataDxfId="205" totalsRowDxfId="204">
+    <tableColumn id="14" xr3:uid="{7DFC35B2-4706-4AE3-A96B-F2996065D7AA}" name="GAS" dataDxfId="206" totalsRowDxfId="205">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{EABEFAC6-21A0-4D0D-814B-53DDA09F13FC}" name="MAG" dataDxfId="203" totalsRowDxfId="202">
+    <tableColumn id="15" xr3:uid="{EABEFAC6-21A0-4D0D-814B-53DDA09F13FC}" name="MAG" dataDxfId="204" totalsRowDxfId="203">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{48811309-731B-4D3E-A293-AB918E5AAA84}" name="VIRAL" dataDxfId="201" totalsRowDxfId="200">
+    <tableColumn id="17" xr3:uid="{48811309-731B-4D3E-A293-AB918E5AAA84}" name="VIRAL" dataDxfId="202" totalsRowDxfId="201">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F998E0FF-9584-4053-837A-904C51049020}" name="CORR" dataDxfId="199" totalsRowDxfId="198">
+    <tableColumn id="13" xr3:uid="{F998E0FF-9584-4053-837A-904C51049020}" name="CORR" dataDxfId="200" totalsRowDxfId="199">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{CD2C3678-91F6-4E1B-8EF0-883C6054EF09}" name="VOID" dataDxfId="197" totalsRowDxfId="196">
+    <tableColumn id="10" xr3:uid="{CD2C3678-91F6-4E1B-8EF0-883C6054EF09}" name="VOID" dataDxfId="198" totalsRowDxfId="197">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7A74E9AA-727D-4FFF-9F30-8F0F56BC2768}" name="TRUE" dataDxfId="195" totalsRowDxfId="194">
+    <tableColumn id="18" xr3:uid="{7A74E9AA-727D-4FFF-9F30-8F0F56BC2768}" name="TRUE" dataDxfId="196" totalsRowDxfId="195">
       <calculatedColumnFormula array="1">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{5C60F2E0-0138-498F-A8DB-5617FA243647}" name="N/A" dataDxfId="193" totalsRowDxfId="192"/>
+    <tableColumn id="11" xr3:uid="{5C60F2E0-0138-498F-A8DB-5617FA243647}" name="N/A" dataDxfId="194" totalsRowDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{33439077-51FD-4559-8B14-6F06E30499DC}" name="FactionInfo" displayName="FactionInfo" ref="A11:R12" headerRowDxfId="191" dataDxfId="190">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{33439077-51FD-4559-8B14-6F06E30499DC}" name="FactionInfo" displayName="FactionInfo" ref="A11:R12" headerRowDxfId="192" dataDxfId="191">
   <autoFilter ref="A11:R12" xr:uid="{33439077-51FD-4559-8B14-6F06E30499DC}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{50793B86-0EAA-4E83-9090-5DBB5B21F946}" name="FACTION" dataDxfId="189" totalsRowDxfId="188"/>
-    <tableColumn id="19" xr3:uid="{E4CB4029-BA21-42B5-AE1D-02800EDC2F29}" name="QUANTA" dataDxfId="187" totalsRowDxfId="186">
+    <tableColumn id="1" xr3:uid="{50793B86-0EAA-4E83-9090-5DBB5B21F946}" name="FACTION" dataDxfId="190" totalsRowDxfId="189"/>
+    <tableColumn id="19" xr3:uid="{E4CB4029-BA21-42B5-AE1D-02800EDC2F29}" name="QUANTA" dataDxfId="188" totalsRowDxfId="187">
       <calculatedColumnFormula array="1">BaseValues[QUANTA]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{36C8BF1C-CC94-401F-B42D-2D3269163FFD}" name="IMPACT" dataDxfId="185" totalsRowDxfId="184">
+    <tableColumn id="2" xr3:uid="{36C8BF1C-CC94-401F-B42D-2D3269163FFD}" name="IMPACT" dataDxfId="186" totalsRowDxfId="185">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[IMPACT],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3C27D35-2706-44F6-9555-61B0F6D4D443}" name="PUNC" dataDxfId="183" totalsRowDxfId="182">
+    <tableColumn id="3" xr3:uid="{B3C27D35-2706-44F6-9555-61B0F6D4D443}" name="PUNC" dataDxfId="184" totalsRowDxfId="183">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[PUNC],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F4D9A0A6-331D-4C9E-8559-E12ADA934C29}" name="SLASH" dataDxfId="181" totalsRowDxfId="180">
+    <tableColumn id="4" xr3:uid="{F4D9A0A6-331D-4C9E-8559-E12ADA934C29}" name="SLASH" dataDxfId="182" totalsRowDxfId="181">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[SLASH],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8D7976C5-E488-4AA2-ACD3-D6DDE095234E}" name="HEAT" dataDxfId="179" totalsRowDxfId="178">
+    <tableColumn id="5" xr3:uid="{8D7976C5-E488-4AA2-ACD3-D6DDE095234E}" name="HEAT" dataDxfId="180" totalsRowDxfId="179">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[HEAT],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{43B2A855-43EA-4B5B-8C4C-094A90C18621}" name="COLD" dataDxfId="177" totalsRowDxfId="176">
+    <tableColumn id="6" xr3:uid="{43B2A855-43EA-4B5B-8C4C-094A90C18621}" name="COLD" dataDxfId="178" totalsRowDxfId="177">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[COLD],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6AA8E83E-0886-4124-A605-69018B4F5CAF}" name="ELEC" dataDxfId="175" totalsRowDxfId="174">
+    <tableColumn id="7" xr3:uid="{6AA8E83E-0886-4124-A605-69018B4F5CAF}" name="ELEC" dataDxfId="176" totalsRowDxfId="175">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[ELEC],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F21013A1-0463-4784-8F50-C75F499DC529}" name="TOXIN" dataDxfId="173" totalsRowDxfId="172">
+    <tableColumn id="8" xr3:uid="{F21013A1-0463-4784-8F50-C75F499DC529}" name="TOXIN" dataDxfId="174" totalsRowDxfId="173">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[TOXIN],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7C0675A0-5B90-4CFB-8016-1689CEA25FBF}" name="BLAST" dataDxfId="171" totalsRowDxfId="170">
+    <tableColumn id="9" xr3:uid="{7C0675A0-5B90-4CFB-8016-1689CEA25FBF}" name="BLAST" dataDxfId="172" totalsRowDxfId="171">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[BLAST],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{007D653B-B2A6-4041-8996-772F81DB6561}" name="RAD" dataDxfId="169" totalsRowDxfId="168">
+    <tableColumn id="12" xr3:uid="{007D653B-B2A6-4041-8996-772F81DB6561}" name="RAD" dataDxfId="170" totalsRowDxfId="169">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[RAD],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{2A40495D-CF10-4CDD-8A1F-BAF58636960B}" name="GAS" dataDxfId="167" totalsRowDxfId="166">
+    <tableColumn id="16" xr3:uid="{2A40495D-CF10-4CDD-8A1F-BAF58636960B}" name="GAS" dataDxfId="168" totalsRowDxfId="167">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[GAS],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A077F0FA-0095-4F42-8CCD-4A6AFEE1497D}" name="MAG" dataDxfId="165" totalsRowDxfId="164">
+    <tableColumn id="14" xr3:uid="{A077F0FA-0095-4F42-8CCD-4A6AFEE1497D}" name="MAG" dataDxfId="166" totalsRowDxfId="165">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[MAG],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{F197187F-7A72-4C14-9448-D512903A219C}" name="VIRAL" dataDxfId="163" totalsRowDxfId="162">
+    <tableColumn id="15" xr3:uid="{F197187F-7A72-4C14-9448-D512903A219C}" name="VIRAL" dataDxfId="164" totalsRowDxfId="163">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[VIRAL],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{533D1553-B264-4101-90A0-3D5A41D8823A}" name="CORR" dataDxfId="161" totalsRowDxfId="160">
+    <tableColumn id="17" xr3:uid="{533D1553-B264-4101-90A0-3D5A41D8823A}" name="CORR" dataDxfId="162" totalsRowDxfId="161">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[CORR],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{06B09C28-FDE1-46A2-A686-1C1EFFBF8378}" name="VOID" dataDxfId="159" totalsRowDxfId="158">
+    <tableColumn id="13" xr3:uid="{06B09C28-FDE1-46A2-A686-1C1EFFBF8378}" name="VOID" dataDxfId="160" totalsRowDxfId="159">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[VOID],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{41483E7F-0438-4FC7-9E0B-B716FB082799}" name="TRUE" dataDxfId="157" totalsRowDxfId="156">
+    <tableColumn id="10" xr3:uid="{41483E7F-0438-4FC7-9E0B-B716FB082799}" name="TRUE" dataDxfId="158" totalsRowDxfId="157">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[TRUE],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{D8377947-8CEF-420C-8745-309F9FB90C5D}" name="N/A" dataDxfId="155"/>
+    <tableColumn id="18" xr3:uid="{D8377947-8CEF-420C-8745-309F9FB90C5D}" name="N/A" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF1B14C7-2ACB-4B3E-AA21-8F8E1E7CF94C}" name="FinalDMG" displayName="FinalDMG" ref="A27:R28" headerRowDxfId="154" dataDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF1B14C7-2ACB-4B3E-AA21-8F8E1E7CF94C}" name="FinalDMG" displayName="FinalDMG" ref="A27:R28" headerRowDxfId="155" dataDxfId="154">
   <autoFilter ref="A27:R28" xr:uid="{DF1B14C7-2ACB-4B3E-AA21-8F8E1E7CF94C}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{7661EA6C-BC60-4D05-9C1F-15981BA8A98B}" name="WEAPON" dataDxfId="152" totalsRowDxfId="151">
+    <tableColumn id="1" xr3:uid="{7661EA6C-BC60-4D05-9C1F-15981BA8A98B}" name="WEAPON" dataDxfId="153" totalsRowDxfId="152">
       <calculatedColumnFormula array="1">BaseValues[WEAPON]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{678F054E-0F50-40A3-AC06-8A6A5EC603EB}" name="QUANTA" dataDxfId="150" totalsRowDxfId="149">
+    <tableColumn id="2" xr3:uid="{678F054E-0F50-40A3-AC06-8A6A5EC603EB}" name="QUANTA" dataDxfId="151" totalsRowDxfId="150">
       <calculatedColumnFormula array="1">BaseValues[QUANTA]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{57208F39-B1F7-439C-B127-5E5FCED00286}" name="IMPACT" dataDxfId="148" totalsRowDxfId="147">
+    <tableColumn id="3" xr3:uid="{57208F39-B1F7-439C-B127-5E5FCED00286}" name="IMPACT" dataDxfId="149" totalsRowDxfId="148">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[IMPACT])*(FactionInfo[IMPACT]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5C8E0E9A-C0F9-48A8-BB2C-B3939E7DAC14}" name="PUNC" dataDxfId="146" totalsRowDxfId="145">
+    <tableColumn id="4" xr3:uid="{5C8E0E9A-C0F9-48A8-BB2C-B3939E7DAC14}" name="PUNC" dataDxfId="147" totalsRowDxfId="146">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[PUNC])*(FactionInfo[PUNC]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8857454B-4E73-4A30-AD30-CF8C77B4C644}" name="SLASH" dataDxfId="144" totalsRowDxfId="143">
+    <tableColumn id="5" xr3:uid="{8857454B-4E73-4A30-AD30-CF8C77B4C644}" name="SLASH" dataDxfId="145" totalsRowDxfId="144">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[SLASH])*(FactionInfo[SLASH]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{09C93641-4128-4F11-A6A6-1C62452DF00F}" name="HEAT" dataDxfId="142" totalsRowDxfId="141">
+    <tableColumn id="6" xr3:uid="{09C93641-4128-4F11-A6A6-1C62452DF00F}" name="HEAT" dataDxfId="143" totalsRowDxfId="142">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[HEAT])*(FactionInfo[HEAT]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{285B3804-A770-4B5E-A634-4B4FD9EAE90B}" name="COLD" dataDxfId="140" totalsRowDxfId="139">
+    <tableColumn id="7" xr3:uid="{285B3804-A770-4B5E-A634-4B4FD9EAE90B}" name="COLD" dataDxfId="141" totalsRowDxfId="140">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[COLD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[COLD])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[COLD])*(FactionInfo[COLD]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EF763390-E62E-4A25-B22E-A5850C58C4D4}" name="ELEC" dataDxfId="138" totalsRowDxfId="137">
+    <tableColumn id="8" xr3:uid="{EF763390-E62E-4A25-B22E-A5850C58C4D4}" name="ELEC" dataDxfId="139" totalsRowDxfId="138">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[ELEC]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[ELEC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[ELEC])*(FactionInfo[ELEC]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{88076855-6F1B-47FE-AF08-4FEC800A17A7}" name="TOXIN" dataDxfId="136" totalsRowDxfId="135">
+    <tableColumn id="9" xr3:uid="{88076855-6F1B-47FE-AF08-4FEC800A17A7}" name="TOXIN" dataDxfId="137" totalsRowDxfId="136">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[TOXIN]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[TOXIN])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[TOXIN])*(FactionInfo[TOXIN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{D50DD866-96F1-4C2E-94CC-138B835BADC8}" name="BLAST" dataDxfId="134" totalsRowDxfId="133">
+    <tableColumn id="12" xr3:uid="{D50DD866-96F1-4C2E-94CC-138B835BADC8}" name="BLAST" dataDxfId="135" totalsRowDxfId="134">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[BLAST]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[BLAST])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[BLAST])*(FactionInfo[BLAST]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{745D2ED4-ED52-4AC3-AF62-D1260AA39A78}" name="RAD" dataDxfId="132" totalsRowDxfId="131">
+    <tableColumn id="16" xr3:uid="{745D2ED4-ED52-4AC3-AF62-D1260AA39A78}" name="RAD" dataDxfId="133" totalsRowDxfId="132">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[RAD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[RAD])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[RAD])*(FactionInfo[RAD]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{70BD75B5-3A2C-4E95-BA4E-441C939A49AE}" name="GAS" dataDxfId="130" totalsRowDxfId="129">
+    <tableColumn id="14" xr3:uid="{70BD75B5-3A2C-4E95-BA4E-441C939A49AE}" name="GAS" dataDxfId="131" totalsRowDxfId="130">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[GAS]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[GAS])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[GAS])*(FactionInfo[GAS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{2BC6EFD8-1FA7-4DFC-9305-E6DA2A6AB50B}" name="MAG" dataDxfId="128" totalsRowDxfId="127">
+    <tableColumn id="15" xr3:uid="{2BC6EFD8-1FA7-4DFC-9305-E6DA2A6AB50B}" name="MAG" dataDxfId="129" totalsRowDxfId="128">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[MAG])*(FactionInfo[MAG]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{846053BC-CC2C-4FE4-8B8E-9D075EB59E32}" name="VIRAL" dataDxfId="126" totalsRowDxfId="125">
+    <tableColumn id="17" xr3:uid="{846053BC-CC2C-4FE4-8B8E-9D075EB59E32}" name="VIRAL" dataDxfId="127" totalsRowDxfId="126">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[VIRAL])*(FactionInfo[VIRAL]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{B3FD166E-66D4-46E8-8C03-C5350D2F00DB}" name="CORR" dataDxfId="124" totalsRowDxfId="123">
+    <tableColumn id="13" xr3:uid="{B3FD166E-66D4-46E8-8C03-C5350D2F00DB}" name="CORR" dataDxfId="125" totalsRowDxfId="124">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[CORR]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[CORR])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[CORR])*(FactionInfo[CORR]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{993447F6-C938-413E-A7C1-70A7CD6ECBA5}" name="VOID" dataDxfId="122" totalsRowDxfId="121">
+    <tableColumn id="10" xr3:uid="{993447F6-C938-413E-A7C1-70A7CD6ECBA5}" name="VOID" dataDxfId="123" totalsRowDxfId="122">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[VOID]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VOID])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[VOID])*(FactionInfo[VOID]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{1577D10B-4C35-4698-A0F7-7516FB8702F7}" name="DMG" dataDxfId="120" totalsRowDxfId="119">
+    <tableColumn id="18" xr3:uid="{1577D10B-4C35-4698-A0F7-7516FB8702F7}" name="DMG" dataDxfId="121" totalsRowDxfId="120">
       <calculatedColumnFormula array="1">ROUND(SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])+SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{14B4E930-A1F0-4AAC-A155-F143B3BDA990}" name="BANE" dataDxfId="118" totalsRowDxfId="117">
+    <tableColumn id="11" xr3:uid="{14B4E930-A1F0-4AAC-A155-F143B3BDA990}" name="BANE" dataDxfId="119" totalsRowDxfId="118">
       <calculatedColumnFormula array="1">ROUND((SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])+SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE])*ModValues[BANE],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8533,61 +8538,61 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D63442A6-FD9A-4ADA-B423-F5568C0540D3}" name="HudValues" displayName="HudValues" ref="A19:R20" headerRowDxfId="116" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D63442A6-FD9A-4ADA-B423-F5568C0540D3}" name="HudValues" displayName="HudValues" ref="A19:R20" headerRowDxfId="117" dataDxfId="116">
   <autoFilter ref="A19:R20" xr:uid="{D63442A6-FD9A-4ADA-B423-F5568C0540D3}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{48C2C412-755E-4B48-8D79-A92CE03BEF47}" name="WEAPON" dataDxfId="114" totalsRowDxfId="113">
+    <tableColumn id="1" xr3:uid="{48C2C412-755E-4B48-8D79-A92CE03BEF47}" name="WEAPON" dataDxfId="115" totalsRowDxfId="114">
       <calculatedColumnFormula array="1">BaseValues[WEAPON]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{13BDA6D7-CCE2-4A09-84AA-C61611B82738}" name="QUANTA" dataDxfId="112" totalsRowDxfId="111">
+    <tableColumn id="2" xr3:uid="{13BDA6D7-CCE2-4A09-84AA-C61611B82738}" name="QUANTA" dataDxfId="113" totalsRowDxfId="112">
       <calculatedColumnFormula array="1">BaseValues[QUANTA]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F797E56E-4352-41A8-B039-E540BE9E2C70}" name="IMPACT" dataDxfId="110" totalsRowDxfId="109">
+    <tableColumn id="3" xr3:uid="{F797E56E-4352-41A8-B039-E540BE9E2C70}" name="IMPACT" dataDxfId="111" totalsRowDxfId="110">
       <calculatedColumnFormula array="1">ROUND((BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8DCDD833-6877-4ADC-B9A5-4109BEDFE0A9}" name="PUNC" dataDxfId="108" totalsRowDxfId="107">
+    <tableColumn id="4" xr3:uid="{8DCDD833-6877-4ADC-B9A5-4109BEDFE0A9}" name="PUNC" dataDxfId="109" totalsRowDxfId="108">
       <calculatedColumnFormula array="1">ROUND((BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{EEDA3E32-2267-43B4-AD8F-36A88DBBD702}" name="SLASH" dataDxfId="106" totalsRowDxfId="105">
+    <tableColumn id="5" xr3:uid="{EEDA3E32-2267-43B4-AD8F-36A88DBBD702}" name="SLASH" dataDxfId="107" totalsRowDxfId="106">
       <calculatedColumnFormula array="1">ROUND((BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{77A0F5DE-EBFF-471B-AC8E-9736FF1E3BB7}" name="HEAT" dataDxfId="104" totalsRowDxfId="103">
+    <tableColumn id="6" xr3:uid="{77A0F5DE-EBFF-471B-AC8E-9736FF1E3BB7}" name="HEAT" dataDxfId="105" totalsRowDxfId="104">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FC719B03-FA4D-4BEA-9F08-7212BB2EC413}" name="COLD" dataDxfId="102" totalsRowDxfId="101">
+    <tableColumn id="7" xr3:uid="{FC719B03-FA4D-4BEA-9F08-7212BB2EC413}" name="COLD" dataDxfId="103" totalsRowDxfId="102">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[COLD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[COLD])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4431E76C-C45F-4658-B676-7AFC238A9BE4}" name="ELEC" dataDxfId="100" totalsRowDxfId="99">
+    <tableColumn id="8" xr3:uid="{4431E76C-C45F-4658-B676-7AFC238A9BE4}" name="ELEC" dataDxfId="101" totalsRowDxfId="100">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[ELEC]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[ELEC])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{95D16F2E-5307-4B7C-95AA-5B2A4320FBCC}" name="TOXIN" dataDxfId="98" totalsRowDxfId="97">
+    <tableColumn id="9" xr3:uid="{95D16F2E-5307-4B7C-95AA-5B2A4320FBCC}" name="TOXIN" dataDxfId="99" totalsRowDxfId="98">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[TOXIN]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[TOXIN])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{874D7A28-8C83-437D-AC2F-E5087EFB2EC3}" name="BLAST" dataDxfId="96" totalsRowDxfId="95">
+    <tableColumn id="12" xr3:uid="{874D7A28-8C83-437D-AC2F-E5087EFB2EC3}" name="BLAST" dataDxfId="97" totalsRowDxfId="96">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[BLAST]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[BLAST])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{5DF62D78-C438-4782-8069-4DD90CACBDDE}" name="RAD" dataDxfId="94" totalsRowDxfId="93">
+    <tableColumn id="16" xr3:uid="{5DF62D78-C438-4782-8069-4DD90CACBDDE}" name="RAD" dataDxfId="95" totalsRowDxfId="94">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[RAD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[RAD])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2216DFFB-D19C-41C1-BCA6-48BF978CD9BC}" name="GAS" dataDxfId="92" totalsRowDxfId="91">
+    <tableColumn id="14" xr3:uid="{2216DFFB-D19C-41C1-BCA6-48BF978CD9BC}" name="GAS" dataDxfId="93" totalsRowDxfId="92">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[GAS]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[GAS])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E0D34BA7-BF0D-45D1-BB93-C02F12EC27A5}" name="MAG" dataDxfId="90" totalsRowDxfId="89">
+    <tableColumn id="15" xr3:uid="{E0D34BA7-BF0D-45D1-BB93-C02F12EC27A5}" name="MAG" dataDxfId="91" totalsRowDxfId="90">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{18FE5F7A-FC18-42EA-AA43-0B8D704B79DF}" name="VIRAL" dataDxfId="88" totalsRowDxfId="87">
+    <tableColumn id="17" xr3:uid="{18FE5F7A-FC18-42EA-AA43-0B8D704B79DF}" name="VIRAL" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EED70621-BCDE-4476-8BDA-3DC7C7C7E4F0}" name="CORR" dataDxfId="86" totalsRowDxfId="85">
+    <tableColumn id="13" xr3:uid="{EED70621-BCDE-4476-8BDA-3DC7C7C7E4F0}" name="CORR" dataDxfId="87" totalsRowDxfId="86">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[CORR]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[CORR])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F360CFAB-4C43-4516-A016-A55AB26FFF89}" name="VOID" dataDxfId="84" totalsRowDxfId="83">
+    <tableColumn id="10" xr3:uid="{F360CFAB-4C43-4516-A016-A55AB26FFF89}" name="VOID" dataDxfId="85" totalsRowDxfId="84">
       <calculatedColumnFormula array="1">ROUND(((BaseValues[VOID]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VOID])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{1E3D39AA-04D1-4E32-A1C0-5847055BEFA3}" name="DMG" dataDxfId="82" totalsRowDxfId="81">
+    <tableColumn id="18" xr3:uid="{1E3D39AA-04D1-4E32-A1C0-5847055BEFA3}" name="DMG" dataDxfId="83" totalsRowDxfId="82">
       <calculatedColumnFormula array="1">ROUND(SUM(HudValues[[#This Row],[IMPACT]:[VOID]])+SUM(HudValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{34D1DDC5-9CC2-4E79-9ED6-D909E92B9CC8}" name="BANE" dataDxfId="80" totalsRowDxfId="79">
+    <tableColumn id="11" xr3:uid="{34D1DDC5-9CC2-4E79-9ED6-D909E92B9CC8}" name="BANE" dataDxfId="81" totalsRowDxfId="80">
       <calculatedColumnFormula array="1">HudValues[[#This Row],[DMG]]*ModValues[BANE]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8596,61 +8601,61 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0973DAB8-4AFD-4D43-8F38-5C78CC5C68A4}" name="GameValues" displayName="GameValues" ref="A23:R24" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0973DAB8-4AFD-4D43-8F38-5C78CC5C68A4}" name="GameValues" displayName="GameValues" ref="A23:R24" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="A23:R24" xr:uid="{0973DAB8-4AFD-4D43-8F38-5C78CC5C68A4}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{B798B903-BCA2-4420-A5F5-8377E6C49741}" name="WEAPON" dataDxfId="34" totalsRowDxfId="35">
+    <tableColumn id="1" xr3:uid="{B798B903-BCA2-4420-A5F5-8377E6C49741}" name="WEAPON" dataDxfId="77" totalsRowDxfId="76">
       <calculatedColumnFormula array="1">BaseValues[WEAPON]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{49FFA8BD-4D0C-4B40-B938-3D713CDC69F7}" name="QUANTA" dataDxfId="32" totalsRowDxfId="33">
+    <tableColumn id="2" xr3:uid="{49FFA8BD-4D0C-4B40-B938-3D713CDC69F7}" name="QUANTA" dataDxfId="75" totalsRowDxfId="74">
       <calculatedColumnFormula array="1">BaseValues[QUANTA]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5D092C06-5763-414F-9C51-EC9805AA4C75}" name="IMPACT" dataDxfId="30" totalsRowDxfId="31">
+    <tableColumn id="3" xr3:uid="{5D092C06-5763-414F-9C51-EC9805AA4C75}" name="IMPACT" dataDxfId="73" totalsRowDxfId="72">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5B520403-5056-43FB-9F70-66AE8EB50841}" name="PUNC" dataDxfId="28" totalsRowDxfId="29">
+    <tableColumn id="4" xr3:uid="{5B520403-5056-43FB-9F70-66AE8EB50841}" name="PUNC" dataDxfId="71" totalsRowDxfId="70">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C55AEFDC-3CCC-42BB-AB4B-D632EE542605}" name="SLASH" dataDxfId="26" totalsRowDxfId="27">
+    <tableColumn id="5" xr3:uid="{C55AEFDC-3CCC-42BB-AB4B-D632EE542605}" name="SLASH" dataDxfId="69" totalsRowDxfId="68">
       <calculatedColumnFormula array="1">ROUND(ROUND(BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7174A6FA-516B-4AD2-931D-38C27EB1BC0F}" name="HEAT" dataDxfId="24" totalsRowDxfId="25">
+    <tableColumn id="6" xr3:uid="{7174A6FA-516B-4AD2-931D-38C27EB1BC0F}" name="HEAT" dataDxfId="67" totalsRowDxfId="66">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9BEC2A05-4891-4F99-A096-03E1624FE095}" name="COLD" dataDxfId="22" totalsRowDxfId="23">
+    <tableColumn id="7" xr3:uid="{9BEC2A05-4891-4F99-A096-03E1624FE095}" name="COLD" dataDxfId="65" totalsRowDxfId="64">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[COLD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[COLD])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3ED51991-15C8-4CA1-BB0A-50FBB3DEF003}" name="ELEC" dataDxfId="20" totalsRowDxfId="21">
+    <tableColumn id="8" xr3:uid="{3ED51991-15C8-4CA1-BB0A-50FBB3DEF003}" name="ELEC" dataDxfId="63" totalsRowDxfId="62">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[ELEC]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[ELEC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F1FC9C06-ADB4-45CB-84D0-13E44F7919F3}" name="TOXIN" dataDxfId="18" totalsRowDxfId="19">
+    <tableColumn id="9" xr3:uid="{F1FC9C06-ADB4-45CB-84D0-13E44F7919F3}" name="TOXIN" dataDxfId="61" totalsRowDxfId="60">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[TOXIN]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[TOXIN])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{54BAFC50-5435-4BC2-9940-12ABD5C506B7}" name="BLAST" dataDxfId="16" totalsRowDxfId="17">
+    <tableColumn id="12" xr3:uid="{54BAFC50-5435-4BC2-9940-12ABD5C506B7}" name="BLAST" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[BLAST]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[BLAST])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{4C379D1C-0905-47EC-B14D-77B6B3C03CE1}" name="RAD" dataDxfId="14" totalsRowDxfId="15">
+    <tableColumn id="16" xr3:uid="{4C379D1C-0905-47EC-B14D-77B6B3C03CE1}" name="RAD" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[RAD]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[RAD])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8D15F3F8-FBDD-44BE-AD4C-E4A4B4510F90}" name="GAS" dataDxfId="12" totalsRowDxfId="13">
+    <tableColumn id="14" xr3:uid="{8D15F3F8-FBDD-44BE-AD4C-E4A4B4510F90}" name="GAS" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[GAS]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[GAS])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{4F8C5E55-EA0E-4C95-BCC9-E19FCF6DCA8A}" name="MAG" dataDxfId="10" totalsRowDxfId="11">
+    <tableColumn id="15" xr3:uid="{4F8C5E55-EA0E-4C95-BCC9-E19FCF6DCA8A}" name="MAG" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{F88009A5-B1DE-4BD4-9047-C650C09D2D3E}" name="VIRAL" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="17" xr3:uid="{F88009A5-B1DE-4BD4-9047-C650C09D2D3E}" name="VIRAL" dataDxfId="51" totalsRowDxfId="50">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{18371472-346F-4D5B-9E1B-15E251CAB919}" name="CORR" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="13" xr3:uid="{18371472-346F-4D5B-9E1B-15E251CAB919}" name="CORR" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[CORR]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[CORR])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{48D55CE6-2A88-4FEC-A32F-6958E469874C}" name="VOID" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="10" xr3:uid="{48D55CE6-2A88-4FEC-A32F-6958E469874C}" name="VOID" dataDxfId="47" totalsRowDxfId="46">
       <calculatedColumnFormula array="1">ROUND(ROUND((BaseValues[VOID]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VOID])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00208949-2227-4833-9F1E-3B70E77979B7}" name="DMG" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="18" xr3:uid="{00208949-2227-4833-9F1E-3B70E77979B7}" name="DMG" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula array="1">ROUND(SUM(GameValues[[#This Row],[IMPACT]:[VOID]])+SUM(GameValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{897019C6-7647-4E2E-AC84-9743258DFB05}" name="BANE" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="11" xr3:uid="{897019C6-7647-4E2E-AC84-9743258DFB05}" name="BANE" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula array="1">ROUND((SUM(GameValues[[#This Row],[IMPACT]:[VOID]])+SUM(GameValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE])*ModValues[BANE],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8659,58 +8664,58 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5997DE-3B7F-4BC8-8136-89E7B95EA52A}" name="WeaponData" displayName="WeaponData" ref="A2:U776" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5997DE-3B7F-4BC8-8136-89E7B95EA52A}" name="WeaponData" displayName="WeaponData" ref="A2:U776" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A2:U776" xr:uid="{1D5997DE-3B7F-4BC8-8136-89E7B95EA52A}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{6E572A45-8AA2-4458-95DC-E32FAA785A6E}" name="WEAPON" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{4AB7A4BF-BADA-4BD7-896E-9A1700DE00B0}" name="DMG" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{A146A45B-3C63-40AB-B5B5-6531E9566734}" name="IMPACT" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{D493C048-3BC4-48FB-BB7B-5F36474E5E77}" name="PUNC" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{B45708B0-68EB-4DA8-80BB-342952107D55}" name="SLASH" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{52A67703-2033-4F83-AAF7-E15FB3CF358C}" name="HEAT" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{F045FEDC-4807-4C4B-965E-12270627A32E}" name="COLD" dataDxfId="70"/>
-    <tableColumn id="13" xr3:uid="{CE69B63B-171A-45AF-9FC5-CD86A531DD24}" name="ELEC" dataDxfId="69"/>
-    <tableColumn id="15" xr3:uid="{67D0D333-A3D7-40F4-B486-7959AFBD3A27}" name="TOXIN" dataDxfId="68"/>
-    <tableColumn id="21" xr3:uid="{15541712-7D95-4DCD-BEC8-EE46387707FB}" name="BLAST" dataDxfId="67"/>
-    <tableColumn id="29" xr3:uid="{36EF4DB4-DD37-4278-AFC3-68073E88DD8D}" name="RAD" dataDxfId="66"/>
-    <tableColumn id="25" xr3:uid="{59C6482A-6B99-484D-B2AB-37DB200CE2CF}" name="GAS" dataDxfId="65"/>
-    <tableColumn id="27" xr3:uid="{6A99EECD-FA7E-45D6-85DF-73144068C74F}" name="MAG" dataDxfId="64"/>
-    <tableColumn id="31" xr3:uid="{62F387D0-B075-4603-A8D1-34A8352D85F4}" name="VIRAL" dataDxfId="63"/>
-    <tableColumn id="23" xr3:uid="{5936C42E-078A-414D-AD77-23F6D0CAD415}" name="CORR" dataDxfId="62"/>
-    <tableColumn id="17" xr3:uid="{3C50BA42-5768-47A1-A3D1-AE176C25E406}" name="VOID" dataDxfId="61"/>
-    <tableColumn id="33" xr3:uid="{8A5AD898-65B0-4EFD-BDF6-F38D34418F1D}" name="CRITCHAN" dataDxfId="60"/>
-    <tableColumn id="34" xr3:uid="{6B33F586-A377-4289-852A-AA8427F6582E}" name="CRITMULT" dataDxfId="59"/>
-    <tableColumn id="37" xr3:uid="{E24F4E5D-BBCB-49E3-880E-6949267789EA}" name="STATCHAN" dataDxfId="58"/>
-    <tableColumn id="35" xr3:uid="{FAEC12C3-E007-4016-AB86-318E6A3EA857}" name="FIRERATE" dataDxfId="57"/>
-    <tableColumn id="36" xr3:uid="{82FC1AC8-7C0F-4B5B-91B1-7B76FF9DA8E6}" name="MULTI" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{6E572A45-8AA2-4458-95DC-E32FAA785A6E}" name="WEAPON" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{4AB7A4BF-BADA-4BD7-896E-9A1700DE00B0}" name="DMG" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{A146A45B-3C63-40AB-B5B5-6531E9566734}" name="IMPACT" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{D493C048-3BC4-48FB-BB7B-5F36474E5E77}" name="PUNC" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{B45708B0-68EB-4DA8-80BB-342952107D55}" name="SLASH" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{52A67703-2033-4F83-AAF7-E15FB3CF358C}" name="HEAT" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{F045FEDC-4807-4C4B-965E-12270627A32E}" name="COLD" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{CE69B63B-171A-45AF-9FC5-CD86A531DD24}" name="ELEC" dataDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{67D0D333-A3D7-40F4-B486-7959AFBD3A27}" name="TOXIN" dataDxfId="31"/>
+    <tableColumn id="21" xr3:uid="{15541712-7D95-4DCD-BEC8-EE46387707FB}" name="BLAST" dataDxfId="30"/>
+    <tableColumn id="29" xr3:uid="{36EF4DB4-DD37-4278-AFC3-68073E88DD8D}" name="RAD" dataDxfId="29"/>
+    <tableColumn id="25" xr3:uid="{59C6482A-6B99-484D-B2AB-37DB200CE2CF}" name="GAS" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{6A99EECD-FA7E-45D6-85DF-73144068C74F}" name="MAG" dataDxfId="27"/>
+    <tableColumn id="31" xr3:uid="{62F387D0-B075-4603-A8D1-34A8352D85F4}" name="VIRAL" dataDxfId="26"/>
+    <tableColumn id="23" xr3:uid="{5936C42E-078A-414D-AD77-23F6D0CAD415}" name="CORR" dataDxfId="25"/>
+    <tableColumn id="17" xr3:uid="{3C50BA42-5768-47A1-A3D1-AE176C25E406}" name="VOID" dataDxfId="24"/>
+    <tableColumn id="33" xr3:uid="{8A5AD898-65B0-4EFD-BDF6-F38D34418F1D}" name="CRITCHAN" dataDxfId="23"/>
+    <tableColumn id="34" xr3:uid="{6B33F586-A377-4289-852A-AA8427F6582E}" name="CRITMULT" dataDxfId="22"/>
+    <tableColumn id="37" xr3:uid="{E24F4E5D-BBCB-49E3-880E-6949267789EA}" name="STATCHAN" dataDxfId="21"/>
+    <tableColumn id="35" xr3:uid="{FAEC12C3-E007-4016-AB86-318E6A3EA857}" name="FIRERATE" dataDxfId="20"/>
+    <tableColumn id="36" xr3:uid="{82FC1AC8-7C0F-4B5B-91B1-7B76FF9DA8E6}" name="MULTI" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E3C113C8-452C-4DEA-8F9A-781C23107A99}" name="FactionData" displayName="FactionData" ref="A2:P13" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E3C113C8-452C-4DEA-8F9A-781C23107A99}" name="FactionData" displayName="FactionData" ref="A2:P13" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:P13" xr:uid="{1D5997DE-3B7F-4BC8-8136-89E7B95EA52A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P3">
     <sortCondition ref="A2:A3"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{35A3619D-5AD7-4DE1-8E32-60145934C907}" name="FACTION" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{BD9C0D82-D946-4EFA-992A-0DB019A96366}" name="IMPACT" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{D058F778-1482-4AF1-BA2D-9DFAE21C841D}" name="PUNC" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{E37129ED-76D3-4096-A4E7-7B820B8EEED3}" name="SLASH" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{A7A0A4A8-C45D-4F7B-AC54-2777CA0339D6}" name="HEAT" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{EA5EEEA5-7180-444D-9CFE-84D8EE0B151A}" name="COLD" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{17B29219-66E1-4C1F-8155-7A145E3F2990}" name="ELEC" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{BC14516B-6FE2-4FA0-ABC1-76883A429D80}" name="TOXIN" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{E7843E46-6996-49FA-88A9-AE7CBFBE1A11}" name="BLAST" dataDxfId="45"/>
-    <tableColumn id="21" xr3:uid="{F1F99C44-A949-4341-A0A6-B6683EB16415}" name="RAD" dataDxfId="44"/>
-    <tableColumn id="29" xr3:uid="{5DB1AB39-8E0A-44C2-ACDA-64B8A045410D}" name="GAS" dataDxfId="43"/>
-    <tableColumn id="25" xr3:uid="{70A69EDA-3D0F-45DA-B0E4-9EEDBC7AB806}" name="MAG" dataDxfId="42"/>
-    <tableColumn id="27" xr3:uid="{71FB4ACE-DC9C-4DEC-98E9-75CC299FE611}" name="VIRAL" dataDxfId="41"/>
-    <tableColumn id="31" xr3:uid="{A65089F8-8943-413D-BF2F-7854E32B56CF}" name="CORR" dataDxfId="40"/>
-    <tableColumn id="23" xr3:uid="{F96C3197-1EFD-4055-9A8A-4723273EB523}" name="VOID" dataDxfId="39"/>
-    <tableColumn id="17" xr3:uid="{AD1A12A7-231D-4888-82CB-A5931B0073DF}" name="TRUE" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{35A3619D-5AD7-4DE1-8E32-60145934C907}" name="FACTION" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{BD9C0D82-D946-4EFA-992A-0DB019A96366}" name="IMPACT" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{D058F778-1482-4AF1-BA2D-9DFAE21C841D}" name="PUNC" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E37129ED-76D3-4096-A4E7-7B820B8EEED3}" name="SLASH" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{A7A0A4A8-C45D-4F7B-AC54-2777CA0339D6}" name="HEAT" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{EA5EEEA5-7180-444D-9CFE-84D8EE0B151A}" name="COLD" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{17B29219-66E1-4C1F-8155-7A145E3F2990}" name="ELEC" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{BC14516B-6FE2-4FA0-ABC1-76883A429D80}" name="TOXIN" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{E7843E46-6996-49FA-88A9-AE7CBFBE1A11}" name="BLAST" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{F1F99C44-A949-4341-A0A6-B6683EB16415}" name="RAD" dataDxfId="7"/>
+    <tableColumn id="29" xr3:uid="{5DB1AB39-8E0A-44C2-ACDA-64B8A045410D}" name="GAS" dataDxfId="6"/>
+    <tableColumn id="25" xr3:uid="{70A69EDA-3D0F-45DA-B0E4-9EEDBC7AB806}" name="MAG" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{71FB4ACE-DC9C-4DEC-98E9-75CC299FE611}" name="VIRAL" dataDxfId="4"/>
+    <tableColumn id="31" xr3:uid="{A65089F8-8943-413D-BF2F-7854E32B56CF}" name="CORR" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{F96C3197-1EFD-4055-9A8A-4723273EB523}" name="VOID" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{AD1A12A7-231D-4888-82CB-A5931B0073DF}" name="TRUE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9001,8 +9006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F502D0-1D0E-452B-9AC0-555D67D1C777}">
   <dimension ref="A1:AD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9029,48 +9034,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="49.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>774</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="31"/>
     </row>
     <row r="2" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>793</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="25"/>
     </row>
     <row r="3" spans="1:30" s="2" customFormat="1" ht="23.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
@@ -9127,27 +9132,30 @@
       <c r="R3" s="8" t="s">
         <v>776</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>821</v>
+      </c>
       <c r="AD3" s="4"/>
     </row>
     <row r="4" spans="1:30" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>280</v>
+        <v>461</v>
       </c>
       <c r="B4" s="6">
         <f>BaseValues[[#This Row],[TOTAL]]/16</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C4" s="6">
         <f>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[IMPACT],0)</f>
-        <v>5.7600002000000003</v>
+        <v>4</v>
       </c>
       <c r="D4" s="6">
         <f>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[PUNC],0)</f>
-        <v>6.7199998000000001</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6">
         <f>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[SLASH],0)</f>
-        <v>3.5200005000000001</v>
+        <v>12</v>
       </c>
       <c r="F4" s="6">
         <f>_xlfn.XLOOKUP(BaseValues[[#This Row],[WEAPON]],WeaponData[WEAPON],WeaponData[HEAT],0)</f>
@@ -9195,11 +9203,11 @@
       </c>
       <c r="Q4" s="6">
         <f>SUM(BaseValues[[#This Row],[IMPACT]:[VOID]])</f>
-        <v>16.000000499999999</v>
+        <v>20</v>
       </c>
       <c r="R4" s="10">
         <f>ROUND(BaseValues[[#This Row],[TOTAL]],0)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9223,26 +9231,26 @@
       <c r="R5" s="18"/>
     </row>
     <row r="6" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>794</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="37"/>
     </row>
     <row r="7" spans="1:30" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -9301,20 +9309,18 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="str" cm="1">
-        <f t="array" ref="A8">BaseValues[WEAPON]</f>
-        <v>Baza Prime</v>
+      <c r="A8" s="9">
+        <v>0</v>
       </c>
       <c r="B8" s="6" cm="1">
         <f t="array" ref="B8">ROUND(BaseValues[QUANTA],2)</f>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
       </c>
       <c r="D8" s="6">
-        <f>1.2</f>
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -9341,8 +9347,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="6">
-        <f>0.9+0.9</f>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="N8" s="6">
         <v>0</v>
@@ -9354,54 +9359,53 @@
         <v>0</v>
       </c>
       <c r="Q8" s="6">
-        <f>1.65</f>
-        <v>1.65</v>
+        <v>0</v>
       </c>
       <c r="R8" s="10">
         <v>1.3</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="33"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="34"/>
     </row>
     <row r="10" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="35" t="s">
         <v>808</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="37"/>
     </row>
     <row r="11" spans="1:30" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -9461,15 +9465,15 @@
     </row>
     <row r="12" spans="1:30" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B12" s="6" cm="1">
         <f t="array" ref="B12">BaseValues[QUANTA]</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C12" s="6" cm="1">
         <f t="array" ref="C12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[IMPACT],0)</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6" cm="1">
         <f t="array" ref="D12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[PUNC],0)</f>
@@ -9477,11 +9481,11 @@
       </c>
       <c r="E12" s="6" cm="1">
         <f t="array" ref="E12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[SLASH],0)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F12" s="6" cm="1">
         <f t="array" ref="F12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[HEAT],0)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G12" s="6" cm="1">
         <f t="array" ref="G12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[COLD],0)</f>
@@ -9517,7 +9521,7 @@
       </c>
       <c r="O12" s="6" cm="1">
         <f t="array" ref="O12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[CORR],0)</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="P12" s="6" cm="1">
         <f t="array" ref="P12">_xlfn.XLOOKUP(FactionInfo[[#This Row],[FACTION]],FactionData[[FACTION]:[FACTION]],FactionData[VOID],0)</f>
@@ -9532,46 +9536,46 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="28"/>
     </row>
     <row r="14" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="35" t="s">
         <v>811</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" spans="1:30" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
@@ -9631,117 +9635,117 @@
     </row>
     <row r="16" spans="1:30" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
-        <v>389</v>
+        <v>0</v>
       </c>
       <c r="B16" s="6" cm="1">
         <f t="array" ref="B16">BaseValues[QUANTA]</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C16" s="6" cm="1">
         <f t="array" ref="C16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="D16" s="6" cm="1">
         <f t="array" ref="D16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="E16" s="6" cm="1">
         <f t="array" ref="E16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="F16" s="6" cm="1">
         <f t="array" ref="F16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="G16" s="6" cm="1">
         <f t="array" ref="G16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="H16" s="6" cm="1">
         <f t="array" ref="H16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="I16" s="6" cm="1">
         <f t="array" ref="I16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="J16" s="6" cm="1">
         <f t="array" ref="J16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="K16" s="6" cm="1">
         <f t="array" ref="K16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="L16" s="6" cm="1">
         <f t="array" ref="L16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6" cm="1">
         <f t="array" ref="M16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="N16" s="6" cm="1">
         <f t="array" ref="N16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="O16" s="6" cm="1">
         <f t="array" ref="O16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="P16" s="6" cm="1">
         <f t="array" ref="P16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="6" cm="1">
         <f t="array" ref="Q16">0.9*SQRT(ArmorMOD[[ARMOR]:[ARMOR]]/2700)</f>
-        <v>0.34161381705077448</v>
+        <v>0</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="33"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="34"/>
     </row>
     <row r="18" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="35" t="s">
         <v>792</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" spans="1:21" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -9802,23 +9806,23 @@
     <row r="20" spans="1:21" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="str" cm="1">
         <f t="array" ref="A20">BaseValues[WEAPON]</f>
-        <v>Baza Prime</v>
+        <v>Kuva Kohm</v>
       </c>
       <c r="B20" s="6" cm="1">
         <f t="array" ref="B20">BaseValues[QUANTA]</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C20" s="12" cm="1">
         <f t="array" ref="C20">ROUND((BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
-        <v>5.7600001799999996</v>
+        <v>4</v>
       </c>
       <c r="D20" s="12" cm="1">
         <f t="array" ref="D20">ROUND((BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
-        <v>14.780000461874998</v>
+        <v>4</v>
       </c>
       <c r="E20" s="12" cm="1">
         <f t="array" ref="E20">ROUND((BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
-        <v>3.5200001099999998</v>
+        <v>12</v>
       </c>
       <c r="F20" s="12" cm="1">
         <f t="array" ref="F20">ROUND(((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
@@ -9850,7 +9854,7 @@
       </c>
       <c r="M20" s="12" cm="1">
         <f t="array" ref="M20">ROUND(((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
-        <v>28.800000899999997</v>
+        <v>0</v>
       </c>
       <c r="N20" s="12" cm="1">
         <f t="array" ref="N20">ROUND(((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]]),2)*BaseValues[[QUANTA]:[QUANTA]]</f>
@@ -9866,54 +9870,54 @@
       </c>
       <c r="Q20" s="6" cm="1">
         <f t="array" ref="Q20">ROUND(SUM(HudValues[[#This Row],[IMPACT]:[VOID]])+SUM(HudValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],1)</f>
-        <v>140.1</v>
+        <v>20</v>
       </c>
       <c r="R20" s="10" cm="1">
         <f t="array" ref="R20">HudValues[[#This Row],[DMG]]*ModValues[BANE]</f>
-        <v>182.13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="33"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="34"/>
     </row>
     <row r="22" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="23" t="s">
         <v>791</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="25"/>
     </row>
     <row r="23" spans="1:21" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -9974,23 +9978,23 @@
     <row r="24" spans="1:21" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="str" cm="1">
         <f t="array" ref="A24">BaseValues[WEAPON]</f>
-        <v>Baza Prime</v>
+        <v>Kuva Kohm</v>
       </c>
       <c r="B24" s="6" cm="1">
         <f t="array" ref="B24">BaseValues[QUANTA]</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C24" s="6" cm="1">
         <f t="array" ref="C24">ROUND(ROUND(BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="D24" s="6" cm="1">
         <f t="array" ref="D24">ROUND(ROUND(BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="E24" s="6" cm="1">
         <f t="array" ref="E24">ROUND(ROUND(BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
-        <v>4</v>
+        <v>12.5</v>
       </c>
       <c r="F24" s="6" cm="1">
         <f t="array" ref="F24">ROUND(ROUND((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
@@ -10022,7 +10026,7 @@
       </c>
       <c r="M24" s="6" cm="1">
         <f t="array" ref="M24">ROUND(ROUND((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N24" s="6" cm="1">
         <f t="array" ref="N24">ROUND(ROUND((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)</f>
@@ -10038,11 +10042,11 @@
       </c>
       <c r="Q24" s="6" cm="1">
         <f t="array" ref="Q24">ROUND(SUM(GameValues[[#This Row],[IMPACT]:[VOID]])+SUM(GameValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],0)</f>
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="R24" s="10" cm="1">
         <f t="array" ref="R24">ROUND((SUM(GameValues[[#This Row],[IMPACT]:[VOID]])+SUM(GameValues[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE])*ModValues[BANE],0)</f>
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="T24" s="19" t="s">
         <v>819</v>
@@ -10052,46 +10056,46 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="27"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="28"/>
     </row>
     <row r="26" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="23" t="s">
         <v>809</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="25"/>
     </row>
     <row r="27" spans="1:21" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
@@ -10152,23 +10156,23 @@
     <row r="28" spans="1:21" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="str" cm="1">
         <f t="array" ref="A28">BaseValues[WEAPON]</f>
-        <v>Baza Prime</v>
+        <v>Kuva Kohm</v>
       </c>
       <c r="B28" s="6" cm="1">
         <f t="array" ref="B28">BaseValues[QUANTA]</f>
-        <v>1.0000000312499999</v>
+        <v>1.25</v>
       </c>
       <c r="C28" s="6" cm="1">
         <f t="array" ref="C28">ROUND(ROUND(BaseValues[IMPACT]*(1+ModValues[IMPACT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[IMPACT])*(FactionInfo[IMPACT]))</f>
-        <v>5.9254756465430294</v>
+        <v>3.75</v>
       </c>
       <c r="D28" s="6" cm="1">
         <f t="array" ref="D28">ROUND(ROUND(BaseValues[PUNC]*(1+ModValues[PUNC])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[PUNC])*(FactionInfo[PUNC]))</f>
-        <v>9.8757927442383817</v>
+        <v>3.75</v>
       </c>
       <c r="E28" s="6" cm="1">
         <f t="array" ref="E28">ROUND(ROUND(BaseValues[SLASH]*(1+ModValues[SLASH])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[SLASH])*(FactionInfo[SLASH]))</f>
-        <v>2.6335447317969018</v>
+        <v>18.75</v>
       </c>
       <c r="F28" s="6" cm="1">
         <f t="array" ref="F28">ROUND(ROUND((BaseValues[HEAT]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[HEAT])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[HEAT])*(FactionInfo[HEAT]))</f>
@@ -10200,7 +10204,7 @@
       </c>
       <c r="M28" s="6" cm="1">
         <f t="array" ref="M28">ROUND(ROUND((BaseValues[MAG]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[MAG])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[MAG])*(FactionInfo[MAG]))</f>
-        <v>19.093199305527538</v>
+        <v>0</v>
       </c>
       <c r="N28" s="6" cm="1">
         <f t="array" ref="N28">ROUND(ROUND((BaseValues[VIRAL]+BaseValues[[TOTAL]:[TOTAL]]*ModValues[VIRAL])/BaseValues[[QUANTA]:[QUANTA]],0)*BaseValues[[QUANTA]:[QUANTA]],3)*((1-ArmorMOD[VIRAL])*(FactionInfo[VIRAL]))</f>
@@ -10216,38 +10220,38 @@
       </c>
       <c r="Q28" s="6" cm="1">
         <f t="array" ref="Q28">ROUND(SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])+SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE],0)</f>
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="R28" s="10" cm="1">
         <f t="array" ref="R28">ROUND((SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])+SUM(FinalDMG[[#This Row],[IMPACT]:[VOID]])*ModValues[TRUE])*ModValues[BANE],0)</f>
-        <v>129</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="27"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="28"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="22" t="s">
         <v>812</v>
       </c>
       <c r="E33" s="13">
@@ -10484,8 +10488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30E7E93-3EBB-4074-B47B-ABA8109F867F}">
   <dimension ref="A1:U776"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="H368" sqref="H368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10514,29 +10518,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="11" customFormat="1" ht="49.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>773</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="40"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -60953,24 +60957,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>773</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">

</xml_diff>